<commit_message>
Updated detailed_work_log.xlsx and meeting minutes
</commit_message>
<xml_diff>
--- a/detailed-logs/Group1_detailed_work_log.xlsx
+++ b/detailed-logs/Group1_detailed_work_log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timot_7crl067\Group1-SOEN341_Project_F24\detailed-logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a351198208daf396/Documents/Concordia University/SOEN 341/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62539252-75B5-42C1-A07D-B8BE91A0DA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="786" documentId="8_{7AA3D587-8EB8-43B0-862E-972F18C56F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{937B5815-0F62-4818-8D47-708649F04DC9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BA86BA27-A737-41DB-9963-64DAB31EA9BC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="59">
   <si>
     <t>Work Log</t>
   </si>
@@ -128,7 +128,7 @@
     <t>Familiarized myself with the current codebase that was worked on by Gregory and Alessandro.</t>
   </si>
   <si>
-    <t>Reviewing some html, css and javascript to prepare for future development.</t>
+    <t>Reviewing some html, css and javascript to prepare for future development and code review.</t>
   </si>
   <si>
     <t>Discussed user stories and story points for sprint 1</t>
@@ -156,6 +156,63 @@
   </si>
   <si>
     <t>Added formatting to README.md and created GitHub Issue templates to streamline creation of new User Stories and tasks. Groomed user stories and task descriptions with Nick G.</t>
+  </si>
+  <si>
+    <t>Updated teams meeting minutes for all team members and jotted team meetings</t>
+  </si>
+  <si>
+    <t>Estimated risk and story points for all previous user stories (sprint 1); updated github story format.</t>
+  </si>
+  <si>
+    <t>Reviewed user requirements for sprint 2; created user stories with descriptions, priority/risk levels, and story points; created relevant dev tasks and grouped them under respective user stories; added/updated GitHub issues according to template.</t>
+  </si>
+  <si>
+    <t>Added search students functionality, as well as the option to import a student roster csv and create teams based on that</t>
+  </si>
+  <si>
+    <t>Pair programmed with Greg to implement get and post routes for student assessment funtionality to create evaluations in database</t>
+  </si>
+  <si>
+    <t>Pair programmed with Olivier to implement get and post routes for student assessment funtionality to create evaluations in database</t>
+  </si>
+  <si>
+    <t>added html and css for navbar and peer assessment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paired programming with nico, finishing up the frontend </t>
+  </si>
+  <si>
+    <t>Pair programmed with alessandro to implement print 2 front end</t>
+  </si>
+  <si>
+    <t>Created 2 acceptance tests.</t>
+  </si>
+  <si>
+    <t>Fixed merge conflicts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updated descriptions to tasks in issues </t>
+  </si>
+  <si>
+    <t>Researched CI/CD workflow setup for GitHub and options for Node.js automated testing that are simple to use. Selected Jest as the top candidate for automated testing.</t>
+  </si>
+  <si>
+    <t>Created basic GitHub workflow YAML script for Node.js CI that is triggered upon pushes and pull requests to any branch. Built upon the script to checkout code to a GitHub workspace, install dependencies, and run a basic assertion test.</t>
+  </si>
+  <si>
+    <t>Reworked the testing models to be automated with Jest. Debugged issues with open handles revealed by Jest tests. Added basic test for the /register GET route. Will add more comprehensive route testing in the future.</t>
+  </si>
+  <si>
+    <t>Added Jest tests for middleware function validation.</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
   </si>
 </sst>
 </file>
@@ -166,7 +223,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,6 +244,12 @@
       <name val="Aptos Display"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -196,7 +259,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -243,77 +306,88 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="18">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -327,85 +401,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="h:mm;@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="h:mm;@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -427,16 +422,12 @@
         <right style="thin">
           <color rgb="FF000000"/>
         </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -449,24 +440,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -479,9 +453,150 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="h:mm;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="h:mm;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -502,12 +617,6 @@
           <color rgb="FF000000"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -528,20 +637,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{81D9EA1B-829C-4D30-A523-5D4F583CA2B9}" name="Table2" displayName="Table2" ref="A2:F31" totalsRowCount="1" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="A2:F30" xr:uid="{81D9EA1B-829C-4D30-A523-5D4F583CA2B9}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F30">
-    <sortCondition ref="A2:A30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{81D9EA1B-829C-4D30-A523-5D4F583CA2B9}" name="Table2" displayName="Table2" ref="A2:G48" totalsRowCount="1" headerRowDxfId="10" dataDxfId="8" totalsRowDxfId="9" tableBorderDxfId="17">
+  <autoFilter ref="A2:G47" xr:uid="{81D9EA1B-829C-4D30-A523-5D4F583CA2B9}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F47">
+    <sortCondition ref="A2:A47"/>
   </sortState>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8D87F16F-6F7B-481C-828D-095856E5E66A}" name="Date" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{1ECAAC90-4FBC-4BDC-B32C-7594F6758112}" name="Team Member" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{D332DE99-9289-488C-95E0-24A7927B9EFE}" name="Activity Description" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{B4AA94E3-0BF5-4AA5-BB8E-ADCF20C768BD}" name="Start Time" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{EB47D0FC-9545-4D44-A955-6F98F9CE63B1}" name="End Time" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{CA2E9783-4F57-4221-B2B7-6044EEA23AA6}" name="Time Spent (hrs)" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0">
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{8D87F16F-6F7B-481C-828D-095856E5E66A}" name="Date" dataDxfId="16" totalsRowDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{1ECAAC90-4FBC-4BDC-B32C-7594F6758112}" name="Team Member" dataDxfId="15" totalsRowDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{D332DE99-9289-488C-95E0-24A7927B9EFE}" name="Activity Description" dataDxfId="14" totalsRowDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{B4AA94E3-0BF5-4AA5-BB8E-ADCF20C768BD}" name="Start Time" dataDxfId="13" totalsRowDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{EB47D0FC-9545-4D44-A955-6F98F9CE63B1}" name="End Time" dataDxfId="12" totalsRowDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{CA2E9783-4F57-4221-B2B7-6044EEA23AA6}" name="Time Spent (hrs)" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="1">
       <calculatedColumnFormula>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="7" xr3:uid="{CE2ACD24-D177-4461-B901-62611BA777E5}" name="Sprint" dataDxfId="7" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -864,57 +974,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE00B9A-3758-45EA-AA57-0C9A801C6022}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31:G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.88671875" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.88671875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" style="5" customWidth="1"/>
+    <col min="7" max="9" width="8.88671875" style="5"/>
+    <col min="10" max="10" width="9.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="5"/>
+    <col min="12" max="12" width="9.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16">
+      <c r="G2" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="9">
         <v>45551</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="10">
@@ -923,21 +1039,24 @@
       <c r="E3" s="10">
         <v>0.78125</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="11">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>0.75</v>
       </c>
-      <c r="J3" s="8"/>
-      <c r="L3" s="8"/>
-    </row>
-    <row r="4" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16">
+      <c r="G3" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="K3" s="12"/>
+      <c r="M3" s="12"/>
+    </row>
+    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="9">
         <v>45552</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="10">
@@ -946,21 +1065,24 @@
       <c r="E4" s="10">
         <v>0.75</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="11">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>0.99999999999999911</v>
       </c>
-      <c r="J4" s="8"/>
-      <c r="L4" s="8"/>
-    </row>
-    <row r="5" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
+      <c r="G4" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" s="12"/>
+      <c r="M4" s="12"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="13">
         <v>45554</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="10">
@@ -969,21 +1091,24 @@
       <c r="E5" s="10">
         <v>0.77083333333333337</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="11">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>1.5</v>
       </c>
-      <c r="J5" s="8"/>
-      <c r="L5" s="8"/>
-    </row>
-    <row r="6" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16">
+      <c r="G5" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" s="12"/>
+      <c r="M5" s="12"/>
+    </row>
+    <row r="6" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
         <v>45554</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="10">
@@ -992,21 +1117,24 @@
       <c r="E6" s="10">
         <v>0.83333333333333337</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="11">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>1.0000000000000018</v>
       </c>
-      <c r="J6" s="8"/>
-      <c r="L6" s="8"/>
-    </row>
-    <row r="7" spans="1:12" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
+      <c r="G6" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6" s="12"/>
+      <c r="M6" s="12"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
         <v>45554</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="10">
@@ -1015,21 +1143,24 @@
       <c r="E7" s="10">
         <v>0.85416666666666663</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="11">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>0.49999999999999822</v>
       </c>
-      <c r="J7" s="8"/>
-      <c r="L7" s="8"/>
-    </row>
-    <row r="8" spans="1:12" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
+      <c r="G7" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="K7" s="12"/>
+      <c r="M7" s="12"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="13">
         <v>45556</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="10">
@@ -1038,21 +1169,24 @@
       <c r="E8" s="10">
         <v>0.58333333333333337</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="11">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>1.0000000000000018</v>
       </c>
-      <c r="J8" s="8"/>
-      <c r="L8" s="8"/>
-    </row>
-    <row r="9" spans="1:12" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16">
+      <c r="G8" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="K8" s="12"/>
+      <c r="M8" s="12"/>
+    </row>
+    <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
         <v>45557</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="10">
@@ -1061,21 +1195,24 @@
       <c r="E9" s="10">
         <v>0.625</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="11">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>3</v>
       </c>
-      <c r="J9" s="8"/>
-      <c r="L9" s="8"/>
-    </row>
-    <row r="10" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16">
+      <c r="G9" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="K9" s="12"/>
+      <c r="M9" s="12"/>
+    </row>
+    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="9">
         <v>45557</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="10">
@@ -1084,21 +1221,24 @@
       <c r="E10" s="10">
         <v>0.60416666666666663</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="11">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>2.4999999999999991</v>
       </c>
-      <c r="J10" s="8"/>
-      <c r="L10" s="8"/>
-    </row>
-    <row r="11" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
+      <c r="G10" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="K10" s="12"/>
+      <c r="M10" s="12"/>
+    </row>
+    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="13">
         <v>45557</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="10">
@@ -1107,19 +1247,22 @@
       <c r="E11" s="10">
         <v>0.8125</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="11">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16">
+      <c r="G11" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="9">
         <v>45557</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="10">
@@ -1128,19 +1271,22 @@
       <c r="E12" s="10">
         <v>0.95833333333333337</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="11">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>0.50000000000000089</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="16">
+      <c r="G12" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="9">
         <v>45558</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="10">
@@ -1149,19 +1295,22 @@
       <c r="E13" s="10">
         <v>0.54166666666666663</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="11">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>0.99999999999999911</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="16">
+      <c r="G13" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="9">
         <v>45558</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D14" s="10">
@@ -1170,19 +1319,22 @@
       <c r="E14" s="10">
         <v>0.875</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="11">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>2.0000000000000009</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16">
+      <c r="G14" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="9">
         <v>45559</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="10">
@@ -1191,19 +1343,22 @@
       <c r="E15" s="10">
         <v>0.66666666666666663</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="11">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>0.99999999999999911</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16">
+      <c r="G15" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="9">
         <v>45559</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D16" s="10">
@@ -1212,19 +1367,22 @@
       <c r="E16" s="10">
         <v>0.60416666666666663</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="11">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="6">
+      <c r="G16" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="13">
         <v>45559</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="10">
@@ -1233,61 +1391,70 @@
       <c r="E17" s="10">
         <v>0.875</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="11">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>2.0000000000000009</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="7">
+      <c r="G17" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="14">
         <v>45560</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="15">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="15">
         <v>0.79166666666666663</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="16">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>1.9999999999999982</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="7">
+      <c r="G18" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="14">
         <v>45561</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="15">
         <v>0</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="15">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="16">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="6">
+      <c r="G19" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="13">
         <v>45561</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="10">
@@ -1296,19 +1463,22 @@
       <c r="E20" s="10">
         <v>0.83333333333333337</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="11">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>1.0000000000000018</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="6">
+      <c r="G20" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="13">
         <v>45561</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D21" s="10">
@@ -1317,19 +1487,22 @@
       <c r="E21" s="10">
         <v>0.75</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="11">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>0.99999999999999911</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="6">
+      <c r="G21" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="13">
         <v>45561</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D22" s="10">
@@ -1338,19 +1511,22 @@
       <c r="E22" s="10">
         <v>0.875</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="11">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="6">
+      <c r="G22" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="13">
         <v>45561</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D23" s="10">
@@ -1359,19 +1535,22 @@
       <c r="E23" s="10">
         <v>0.70833333333333337</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="11">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>1.0000000000000018</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="6">
+      <c r="G23" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="13">
         <v>45561</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D24" s="10">
@@ -1380,82 +1559,94 @@
       <c r="E24" s="10">
         <v>0.79166666666666663</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="11">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>1.9999999999999982</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="7">
+      <c r="G24" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="14">
         <v>45562</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="15">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="15">
         <v>0.75</v>
       </c>
-      <c r="F25" s="12">
+      <c r="F25" s="16">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>3.9999999999999991</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="7">
+      <c r="G25" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="14">
         <v>45562</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="15">
         <v>0.79166666666666663</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="15">
         <v>0.875</v>
       </c>
-      <c r="F26" s="12">
+      <c r="F26" s="16">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>2.0000000000000009</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="7">
+      <c r="G26" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="14">
         <v>45563</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="15">
         <v>0.5</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="15">
         <v>0.75</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27" s="16">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="6">
+      <c r="G27" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="13">
         <v>45563</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D28" s="10">
@@ -1464,19 +1655,22 @@
       <c r="E28" s="10">
         <v>0.95833333333333337</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28" s="11">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>5.0000000000000009</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="6">
+      <c r="G28" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="13">
         <v>45564</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D29" s="10">
@@ -1485,44 +1679,448 @@
       <c r="E29" s="10">
         <v>0.875</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29" s="11">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>2.0000000000000009</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="7">
+      <c r="G29" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="14">
         <v>45564</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="15">
         <v>0.66666666666666663</v>
       </c>
-      <c r="E30" s="11">
+      <c r="E30" s="15">
         <v>0.83333333333333337</v>
       </c>
-      <c r="F30" s="12">
+      <c r="F30" s="16">
         <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
         <v>4.0000000000000018</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="19">
+      <c r="G30" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="13">
+        <v>45570</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="10">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E31" s="10">
+        <v>0.625</v>
+      </c>
+      <c r="F31" s="11">
+        <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
+        <v>0.99999999999999911</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="13">
+        <v>45578</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="10">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E32" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="F32" s="11">
+        <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
+        <v>0.99999999999999911</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="13">
+        <v>45579</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="E33" s="10">
+        <v>0.875</v>
+      </c>
+      <c r="F33" s="11">
+        <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
+        <v>3</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="13">
+        <v>45587</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="10">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E34" s="10">
+        <v>0.90625</v>
+      </c>
+      <c r="F34" s="11">
+        <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
+        <v>1.7499999999999991</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="13">
+        <v>45590</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="10">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E35" s="10">
+        <v>0.72569444444444442</v>
+      </c>
+      <c r="F35" s="11">
+        <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
+        <v>1.416666666666667</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="13">
+        <v>45590</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D36" s="10">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E36" s="10">
+        <v>0.72569444444444442</v>
+      </c>
+      <c r="F36" s="11">
+        <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
+        <v>1.416666666666667</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="13">
+        <v>45591</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37" s="10">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E37" s="10">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F37" s="11">
+        <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
+        <v>1.9999999999999982</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="13">
+        <v>45592</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D38" s="10">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E38" s="10">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="F38" s="11">
+        <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
+        <v>4.5</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="13">
+        <v>45592</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39" s="10">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E39" s="10">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="F39" s="11">
+        <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
+        <v>4.5</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="13">
+        <v>45592</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D40" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="E40" s="10">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F40" s="11">
+        <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
+        <v>2.0000000000000009</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="13">
+        <v>45592</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" s="10">
+        <v>0.875</v>
+      </c>
+      <c r="E41" s="10">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="F41" s="11">
+        <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
+        <v>1.2500000000000009</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="13">
+        <v>45592</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D42" s="10">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E42" s="10">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="F42" s="11">
+        <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
+        <v>1.5</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="13">
+        <v>45592</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D43" s="10">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E43" s="10">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F43" s="11">
+        <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
+        <v>4.0000000000000018</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="13">
+        <v>45594</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D44" s="10">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="E44" s="10">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F44" s="11">
+        <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
+        <v>5.2500000000000018</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A45" s="13">
+        <v>45595</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="10">
+        <v>0.8125</v>
+      </c>
+      <c r="E45" s="10">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="F45" s="11">
+        <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
+        <v>3.9999999999999991</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="13">
+        <v>45596</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D46" s="10">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E46" s="10">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F46" s="11">
+        <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
+        <v>1.9999999999999996</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="13"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="11" t="str">
+        <f>IF(Table2[[#This Row],[Start Time]]&lt;&gt;"",(Table2[[#This Row],[End Time]]-Table2[[#This Row],[Start Time]]) * 24, "")</f>
+        <v/>
+      </c>
+      <c r="G47" s="16"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="17">
         <f>SUBTOTAL(109,Table2[Time Spent (hrs)])</f>
-        <v>54.75</v>
-      </c>
+        <v>95.333333333333329</v>
+      </c>
+      <c r="G48" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>